<commit_message>
fede 20/06 18.55 pm
</commit_message>
<xml_diff>
--- a/Diccionario de datos.xlsx
+++ b/Diccionario de datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Desktop\PF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EABE7BC-A09C-4902-97EC-15CCBFF48776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E387C2B3-A420-4ABF-AF33-8AA4B32A814B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata-sitios" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,25 @@
     <sheet name="tip.json" sheetId="7" r:id="rId7"/>
     <sheet name="DER" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="298">
   <si>
     <t>Variables</t>
   </si>
@@ -134,9 +147,6 @@
     <t>Longitud geográfica.</t>
   </si>
   <si>
-    <t>Categoría del luga</t>
-  </si>
-  <si>
     <t>Puntuación media</t>
   </si>
   <si>
@@ -179,9 +189,6 @@
     <t>subcategoria</t>
   </si>
   <si>
-    <t>Resultados relacionados</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ejemplos </t>
   </si>
   <si>
@@ -203,9 +210,6 @@
     <t>Pharmacy'</t>
   </si>
   <si>
-    <t xml:space="preserve">4.2, </t>
-  </si>
-  <si>
     <t>'$$'</t>
   </si>
   <si>
@@ -236,13 +240,7 @@
     <t>'https://www.google.com/maps/place//data=!4m2!3m1!1s0x881614ce7c13acb</t>
   </si>
   <si>
-    <t>    b:0x5c7b18bbf6ec4f7e?authuser=-1&amp;hl=en&amp;gl=us'</t>
-  </si>
-  <si>
     <t>URL del lugar en google maps</t>
-  </si>
-  <si>
-    <t>Estado (cerrado-Abierto)</t>
   </si>
   <si>
     <t>numero de reviews</t>
@@ -983,12 +981,168 @@
   <si>
     <t>compliment_photos</t>
   </si>
+  <si>
+    <t>tamaño dato</t>
+  </si>
+  <si>
+    <t>maximo 246 caracteres</t>
+  </si>
+  <si>
+    <t>nulos</t>
+  </si>
+  <si>
+    <t>14 a 297 caracteres</t>
+  </si>
+  <si>
+    <t>22 a 35 caracteres</t>
+  </si>
+  <si>
+    <t>max 110 caracteres</t>
+  </si>
+  <si>
+    <t>2 enteros, 6 decimales</t>
+  </si>
+  <si>
+    <t>negativo, 3 enteros, 6 decimales</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>lista de textos</t>
+  </si>
+  <si>
+    <t>Categoría del lugar (3.895 en total)</t>
+  </si>
+  <si>
+    <t>1 a 5, un decimal</t>
+  </si>
+  <si>
+    <t>max 9.998</t>
+  </si>
+  <si>
+    <t>max 14 categorías, 312 caracteres</t>
+  </si>
+  <si>
+    <t>7 items, 255 caracteres</t>
+  </si>
+  <si>
+    <t>texto</t>
+  </si>
+  <si>
+    <t>4 caracteres</t>
+  </si>
+  <si>
+    <t>Estado (cerrado-Abierto) al momento de tomar el dato</t>
+  </si>
+  <si>
+    <t>max 41 caracteres</t>
+  </si>
+  <si>
+    <t>97-122 caracteres</t>
+  </si>
+  <si>
+    <t>lista de resultados relacionados</t>
+  </si>
+  <si>
+    <t>5 items, 205 caracteres</t>
+  </si>
+  <si>
+    <t>cantidad de datos (sin duplicados)</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>tamaño</t>
+  </si>
+  <si>
+    <t>21 cifras</t>
+  </si>
+  <si>
+    <t>77 caracteres (incluye caracteres extranjeros)</t>
+  </si>
+  <si>
+    <t>Cantidad (sin duplicados)</t>
+  </si>
+  <si>
+    <t>13 cifras</t>
+  </si>
+  <si>
+    <t>del 1 al 5</t>
+  </si>
+  <si>
+    <t>máximo de 8360 caracteres</t>
+  </si>
+  <si>
+    <t>máximo de 5.600 caracteres</t>
+  </si>
+  <si>
+    <t>max 4.041 caracteres</t>
+  </si>
+  <si>
+    <t>22 a 37 caracteres</t>
+  </si>
+  <si>
+    <t>url (varias)</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Offerings</t>
+  </si>
+  <si>
+    <t>Health and safety</t>
+  </si>
+  <si>
+    <t>Activities</t>
+  </si>
+  <si>
+    <t>Amenities</t>
+  </si>
+  <si>
+    <t>Atmosphere</t>
+  </si>
+  <si>
+    <t>Crowd</t>
+  </si>
+  <si>
+    <t>Dining options</t>
+  </si>
+  <si>
+    <t>From the business</t>
+  </si>
+  <si>
+    <t>Getting here</t>
+  </si>
+  <si>
+    <t>Highlights</t>
+  </si>
+  <si>
+    <t>Popular for</t>
+  </si>
+  <si>
+    <t>Recycling</t>
+  </si>
+  <si>
+    <t>1.279 caracteres</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1054,6 +1208,19 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1181,7 +1348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1297,6 +1464,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1602,34 +1790,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="25.88671875" customWidth="1"/>
-    <col min="4" max="5" width="22.5546875" customWidth="1"/>
-    <col min="6" max="6" width="57.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="200.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" customWidth="1"/>
+    <col min="2" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="26"/>
       <c r="E1" s="26"/>
       <c r="F1" s="26"/>
       <c r="G1" s="26"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1637,22 +1833,31 @@
         <v>24</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>38</v>
+        <v>246</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1667,13 +1872,22 @@
         <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G3" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J3" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1688,13 +1902,22 @@
         <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G4" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J4" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1709,13 +1932,22 @@
         <v>19</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="G5" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J5" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1730,18 +1962,27 @@
         <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="G6" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H6" s="13">
+        <v>262864</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J6" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
@@ -1751,18 +1992,27 @@
         <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G7" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="2">
+      <c r="J7" s="2">
         <v>4.1451859999999904E+16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
@@ -1772,14 +2022,23 @@
         <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="G8" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="J8" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1787,24 +2046,33 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>18</v>
+        <v>254</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>19</v>
+        <v>255</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="G9" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H9" s="13">
+        <v>1881</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
@@ -1814,18 +2082,27 @@
         <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="G10" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
@@ -1835,14 +2112,23 @@
         <v>23</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G11" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1850,211 +2136,700 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>18</v>
+        <v>254</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>19</v>
+        <v>261</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="G12" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H12" s="13">
+        <v>263155</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>27</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="G13" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H13" s="13">
+        <v>66506</v>
+      </c>
+      <c r="I13" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13" s="44" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="2" t="s">
-        <v>39</v>
+        <v>120</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
+        <v>261</v>
+      </c>
+      <c r="F14" s="20"/>
+      <c r="G14" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H14" s="13">
+        <v>66506</v>
+      </c>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="20"/>
       <c r="B15" s="20"/>
       <c r="C15" s="2" t="s">
-        <v>40</v>
+        <v>281</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
+        <v>261</v>
+      </c>
+      <c r="F15" s="20"/>
+      <c r="G15" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H15" s="13">
+        <v>66506</v>
+      </c>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="20"/>
       <c r="B16" s="20"/>
       <c r="C16" s="2" t="s">
-        <v>41</v>
+        <v>282</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
+        <v>261</v>
+      </c>
+      <c r="F16" s="20"/>
+      <c r="G16" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H16" s="13">
+        <v>66506</v>
+      </c>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="20"/>
       <c r="B17" s="20"/>
       <c r="C17" s="2" t="s">
-        <v>42</v>
+        <v>283</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="21"/>
+        <v>261</v>
+      </c>
+      <c r="F17" s="20"/>
+      <c r="G17" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H17" s="13">
+        <v>66506</v>
+      </c>
+      <c r="I17" s="45"/>
+      <c r="J17" s="45"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="F18" s="20"/>
+      <c r="G18" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H18" s="13">
+        <v>66506</v>
+      </c>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="2" t="s">
+        <v>284</v>
+      </c>
       <c r="D19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="2"/>
+        <v>261</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H19" s="13">
+        <v>66506</v>
+      </c>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="D20" s="2" t="s">
-        <v>18</v>
+        <v>254</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="2"/>
+      <c r="F20" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="G20" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H20" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="42"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="D21" s="2" t="s">
-        <v>18</v>
+        <v>254</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E22" s="4"/>
-      <c r="G22" t="s">
-        <v>69</v>
-      </c>
+      <c r="F21" s="20"/>
+      <c r="G21" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H21" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="42"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H22" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="42"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H23" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="42"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="20"/>
+      <c r="G24" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H24" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="42"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="20"/>
+      <c r="G25" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H25" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="42"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="20"/>
+      <c r="G26" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H26" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="42"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="20"/>
+      <c r="G27" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H27" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="42"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H28" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="42"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="20"/>
+      <c r="G29" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H29" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="42"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="20"/>
+      <c r="G30" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H30" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="42"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="20"/>
+      <c r="G31" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H31" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="42"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="20"/>
+      <c r="G32" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H32" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="42"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="20"/>
+      <c r="G33" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H33" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="42"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="20"/>
+      <c r="G34" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H34" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="42"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="20"/>
+      <c r="G35" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H35" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="43"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="21"/>
+      <c r="G36" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H36" s="13">
+        <v>52500</v>
+      </c>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="G37" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H37" s="13">
+        <v>63238</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="G38" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H38" s="13">
+        <v>23740</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="G39" s="13">
+        <v>294593</v>
+      </c>
+      <c r="H39" s="13">
+        <v>0</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B1:G1"/>
+  <mergeCells count="9">
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="F13:F19"/>
+    <mergeCell ref="A20:A36"/>
+    <mergeCell ref="B20:B36"/>
+    <mergeCell ref="F20:F36"/>
+    <mergeCell ref="I13:I19"/>
+    <mergeCell ref="J13:J19"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2062,10 +2837,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2074,24 +2849,30 @@
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="84.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.44140625" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="84.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
       <c r="F1" s="27"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2099,37 +2880,54 @@
         <v>24</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>38</v>
+        <v>270</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>273</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+      <c r="F3" s="13">
+        <f>2700000-76277</f>
+        <v>2623723</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -2141,15 +2939,23 @@
         <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+      <c r="F4" s="13">
+        <f t="shared" ref="F4:F11" si="0">2700000-76277</f>
+        <v>2623723</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>25</v>
@@ -2159,15 +2965,23 @@
         <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="12">
+        <v>274</v>
+      </c>
+      <c r="F5" s="13">
+        <f t="shared" si="0"/>
+        <v>2623723</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" s="12">
         <v>1627750414677</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>25</v>
@@ -2177,15 +2991,23 @@
         <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>275</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" si="0"/>
+        <v>2623723</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>26</v>
@@ -2195,68 +3017,110 @@
         <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>276</v>
+      </c>
+      <c r="F7" s="13">
+        <f t="shared" si="0"/>
+        <v>2623723</v>
+      </c>
+      <c r="G7" s="13">
+        <v>1163823</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>280</v>
+      </c>
       <c r="D8" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="0"/>
+        <v>2623723</v>
+      </c>
+      <c r="G8" s="40">
+        <v>2530146</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="28" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F9" s="12">
+        <v>274</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="0"/>
+        <v>2623723</v>
+      </c>
+      <c r="G9" s="13">
+        <v>2386301</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="12">
         <v>628455067818</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29"/>
       <c r="B10" s="20"/>
       <c r="C10" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" si="0"/>
+        <v>2623723</v>
+      </c>
+      <c r="G10" s="13">
+        <v>2386301</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2267,103 +3131,144 @@
         <v>18</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+      <c r="F11" s="13">
+        <f t="shared" si="0"/>
+        <v>2623723</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B1:I1"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="A9:A10"/>
   </mergeCells>
@@ -2394,7 +3299,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
@@ -2410,27 +3315,27 @@
         <v>24</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -2438,18 +3343,18 @@
         <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2457,18 +3362,18 @@
         <v>18</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -2476,18 +3381,18 @@
         <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -2495,18 +3400,18 @@
         <v>18</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -2514,18 +3419,18 @@
         <v>18</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -2533,18 +3438,18 @@
         <v>18</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -2552,7 +3457,7 @@
         <v>20</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G9" s="13">
         <v>377817529521</v>
@@ -2560,10 +3465,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -2571,7 +3476,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G10" s="13">
         <v>-12239612197</v>
@@ -2579,10 +3484,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -2590,18 +3495,18 @@
         <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -2609,7 +3514,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="G12" s="2">
         <v>1198</v>
@@ -2617,10 +3522,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -2628,7 +3533,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G13" s="2">
         <v>1</v>
@@ -2636,42 +3541,42 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="30"/>
       <c r="B15" s="23"/>
       <c r="C15" s="20" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2679,16 +3584,16 @@
       <c r="B16" s="23"/>
       <c r="C16" s="20"/>
       <c r="D16" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -2696,16 +3601,16 @@
       <c r="B17" s="23"/>
       <c r="C17" s="20"/>
       <c r="D17" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -2713,16 +3618,16 @@
       <c r="B18" s="23"/>
       <c r="C18" s="20"/>
       <c r="D18" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2730,24 +3635,24 @@
       <c r="B19" s="24"/>
       <c r="C19" s="21"/>
       <c r="D19" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -2755,21 +3660,21 @@
         <v>18</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="3" t="s">
@@ -2777,31 +3682,31 @@
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="30"/>
       <c r="B22" s="32"/>
       <c r="C22" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F22" s="30" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="30"/>
       <c r="B23" s="32"/>
       <c r="C23" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="3" t="s">
@@ -2809,14 +3714,14 @@
       </c>
       <c r="F23" s="30"/>
       <c r="G23" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="30"/>
       <c r="B24" s="32"/>
       <c r="C24" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="3" t="s">
@@ -2824,14 +3729,14 @@
       </c>
       <c r="F24" s="30"/>
       <c r="G24" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="30"/>
       <c r="B25" s="32"/>
       <c r="C25" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="3" t="s">
@@ -2839,14 +3744,14 @@
       </c>
       <c r="F25" s="30"/>
       <c r="G25" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="30"/>
       <c r="B26" s="32"/>
       <c r="C26" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="3" t="s">
@@ -2854,14 +3759,14 @@
       </c>
       <c r="F26" s="30"/>
       <c r="G26" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="30"/>
       <c r="B27" s="32"/>
       <c r="C27" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="3" t="s">
@@ -2869,7 +3774,7 @@
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2908,7 +3813,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
@@ -2925,75 +3830,75 @@
         <v>2</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E6" s="15">
         <v>4</v>
@@ -3001,50 +3906,50 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E9" s="15">
         <v>0</v>
@@ -3052,16 +3957,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E10" s="15">
         <v>0</v>
@@ -3069,16 +3974,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
@@ -3174,7 +4079,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="27"/>
@@ -3191,22 +4096,22 @@
         <v>24</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>19</v>
@@ -3217,10 +4122,10 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -3236,26 +4141,26 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G5" s="2">
         <v>585</v>
@@ -3263,10 +4168,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
@@ -3274,22 +4179,22 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -3299,14 +4204,14 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -3316,14 +4221,14 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -3333,7 +4238,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>19</v>
@@ -3344,15 +4249,15 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>19</v>
@@ -3363,24 +4268,24 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="G12" s="2">
         <v>52</v>
@@ -3388,33 +4293,33 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -3424,14 +4329,14 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -3441,14 +4346,14 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -3458,14 +4363,14 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -3475,14 +4380,14 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -3492,14 +4397,14 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -3509,14 +4414,14 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -3526,14 +4431,14 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -3543,14 +4448,14 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -3560,14 +4465,14 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -3577,14 +4482,14 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -3612,7 +4517,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="27"/>
@@ -3629,22 +4534,22 @@
         <v>24</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>19</v>
@@ -3655,31 +4560,31 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -3858,7 +4763,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -3875,22 +4780,22 @@
         <v>24</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>19</v>
@@ -3901,15 +4806,15 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>19</v>
@@ -3920,15 +4825,15 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
@@ -3939,45 +4844,45 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
@@ -3995,7 +4900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A3:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
@@ -4013,7 +4918,7 @@
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B3" s="34"/>
     </row>
@@ -4031,10 +4936,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -4049,16 +4954,16 @@
         <v>8</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -4067,16 +4972,16 @@
         <v>7</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -4089,7 +4994,7 @@
         <v>3</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="N10" s="1"/>
     </row>
@@ -4100,10 +5005,10 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N11" s="1"/>
     </row>
@@ -4114,10 +5019,10 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="N12" s="1"/>
     </row>
@@ -4128,10 +5033,10 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="N13" s="1"/>
     </row>
@@ -4142,10 +5047,10 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="11" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="N14" s="1"/>
     </row>
@@ -4156,10 +5061,10 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="17" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="N15" s="1"/>
     </row>
@@ -4169,13 +5074,13 @@
         <v>15</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="N16" s="1"/>
     </row>
@@ -4185,7 +5090,7 @@
         <v>16</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="N17" s="1"/>
     </row>
@@ -4195,46 +5100,46 @@
         <v>17</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="N18" s="1"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="M19" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="N19" s="1"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="M20" s="7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="N20" s="1"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="M21" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="N21" s="1"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="M22" s="7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="N22" s="1"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P25" s="38" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="Q25" s="39"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P26" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
@@ -4246,206 +5151,206 @@
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P28" s="1"/>
       <c r="Q28" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P29" s="1"/>
       <c r="Q29" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G30" s="36" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H30" s="37"/>
       <c r="J30" s="38" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="K30" s="39"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G31" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="J31" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="P31" s="1"/>
       <c r="Q31" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G32" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J32" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="P32" s="1"/>
       <c r="Q32" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="7:17" x14ac:dyDescent="0.3">
       <c r="G33" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="P33" s="1"/>
       <c r="Q33" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="7:17" x14ac:dyDescent="0.3">
       <c r="G34" s="1"/>
       <c r="H34" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="P34" s="1"/>
       <c r="Q34" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="35" spans="7:17" x14ac:dyDescent="0.3">
       <c r="G35" s="1"/>
       <c r="H35" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P35" s="1"/>
       <c r="Q35" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="7:17" x14ac:dyDescent="0.3">
       <c r="G36" s="1"/>
       <c r="H36" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="P36" s="1"/>
       <c r="Q36" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="7:17" x14ac:dyDescent="0.3">
       <c r="G37" s="1"/>
       <c r="H37" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="P37" s="1"/>
       <c r="Q37" s="2" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="7:17" x14ac:dyDescent="0.3">
       <c r="G38" s="1"/>
       <c r="H38" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="J38" s="34" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="K38" s="34"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="39" spans="7:17" x14ac:dyDescent="0.3">
       <c r="G39" s="1"/>
       <c r="H39" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="P39" s="1"/>
       <c r="Q39" s="2" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="40" spans="7:17" x14ac:dyDescent="0.3">
       <c r="J40" s="1"/>
       <c r="K40" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="P40" s="1"/>
       <c r="Q40" s="2" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" spans="7:17" x14ac:dyDescent="0.3">
       <c r="P41" s="1"/>
       <c r="Q41" s="2" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="42" spans="7:17" x14ac:dyDescent="0.3">
       <c r="P42" s="1"/>
       <c r="Q42" s="2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="7:17" x14ac:dyDescent="0.3">
       <c r="P43" s="1"/>
       <c r="Q43" s="2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="44" spans="7:17" x14ac:dyDescent="0.3">
       <c r="P44" s="1"/>
       <c r="Q44" s="2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="45" spans="7:17" x14ac:dyDescent="0.3">
       <c r="P45" s="1"/>
       <c r="Q45" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="46" spans="7:17" x14ac:dyDescent="0.3">
       <c r="P46" s="1"/>
       <c r="Q46" s="2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="47" spans="7:17" x14ac:dyDescent="0.3">
       <c r="P47" s="1"/>
       <c r="Q47" s="2" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fede 21/06 16 pm
</commit_message>
<xml_diff>
--- a/Diccionario de datos.xlsx
+++ b/Diccionario de datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Desktop\PF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E387C2B3-A420-4ABF-AF33-8AA4B32A814B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308C7330-550B-452B-9591-0AD5D8453647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata-sitios" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="299">
   <si>
     <t>Variables</t>
   </si>
@@ -988,9 +988,6 @@
     <t>maximo 246 caracteres</t>
   </si>
   <si>
-    <t>nulos</t>
-  </si>
-  <si>
     <t>14 a 297 caracteres</t>
   </si>
   <si>
@@ -1048,9 +1045,6 @@
     <t>5 items, 205 caracteres</t>
   </si>
   <si>
-    <t>cantidad de datos (sin duplicados)</t>
-  </si>
-  <si>
     <t>4.2</t>
   </si>
   <si>
@@ -1063,9 +1057,6 @@
     <t>77 caracteres (incluye caracteres extranjeros)</t>
   </si>
   <si>
-    <t>Cantidad (sin duplicados)</t>
-  </si>
-  <si>
     <t>13 cifras</t>
   </si>
   <si>
@@ -1136,6 +1127,18 @@
   </si>
   <si>
     <t>1.279 caracteres</t>
+  </si>
+  <si>
+    <t>Datos originales</t>
+  </si>
+  <si>
+    <t>Datos sin duplicados</t>
+  </si>
+  <si>
+    <t>Nulos</t>
+  </si>
+  <si>
+    <t>Datos netos (sin nulos</t>
   </si>
 </sst>
 </file>
@@ -1348,7 +1351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1402,6 +1405,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1411,20 +1423,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1440,6 +1455,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1465,26 +1489,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1790,10 +1802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1802,30 +1814,32 @@
     <col min="2" max="3" width="20.44140625" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.44140625" customWidth="1"/>
+    <col min="6" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="9" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1845,19 +1859,25 @@
         <v>246</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>268</v>
+        <v>295</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>248</v>
+        <v>296</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1875,19 +1895,26 @@
         <v>247</v>
       </c>
       <c r="G3" s="13">
+        <v>297293</v>
+      </c>
+      <c r="H3" s="13">
         <v>294593</v>
       </c>
-      <c r="H3" s="13">
+      <c r="I3" s="13">
         <v>0</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="13">
+        <f>H3-I3</f>
+        <v>294593</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1902,22 +1929,29 @@
         <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G4" s="13">
+        <v>297293</v>
+      </c>
+      <c r="H4" s="13">
         <v>294593</v>
       </c>
-      <c r="H4" s="13">
+      <c r="I4" s="13">
         <v>0</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="13">
+        <f t="shared" ref="J4:J39" si="0">H4-I4</f>
+        <v>294593</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1932,22 +1966,29 @@
         <v>19</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G5" s="13">
+        <v>297293</v>
+      </c>
+      <c r="H5" s="13">
         <v>294593</v>
       </c>
-      <c r="H5" s="13">
+      <c r="I5" s="13">
         <v>0</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="13">
+        <f t="shared" si="0"/>
+        <v>294593</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1962,22 +2003,29 @@
         <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G6" s="13">
+        <v>297293</v>
+      </c>
+      <c r="H6" s="13">
         <v>294593</v>
       </c>
-      <c r="H6" s="13">
+      <c r="I6" s="13">
         <v>262864</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="13">
+        <f t="shared" si="0"/>
+        <v>31729</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1992,22 +2040,29 @@
         <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G7" s="13">
+        <v>297293</v>
+      </c>
+      <c r="H7" s="13">
         <v>294593</v>
       </c>
-      <c r="H7" s="13">
+      <c r="I7" s="13">
         <v>0</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="13">
+        <f t="shared" si="0"/>
+        <v>294593</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="2">
+      <c r="L7" s="2">
         <v>4.1451859999999904E+16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2022,22 +2077,29 @@
         <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G8" s="13">
+        <v>297293</v>
+      </c>
+      <c r="H8" s="13">
         <v>294593</v>
       </c>
-      <c r="H8" s="13">
+      <c r="I8" s="13">
         <v>0</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="13">
+        <f t="shared" si="0"/>
+        <v>294593</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -2046,28 +2108,35 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G9" s="13">
+        <v>297293</v>
+      </c>
+      <c r="H9" s="13">
+        <v>294593</v>
+      </c>
+      <c r="I9" s="13">
+        <v>1881</v>
+      </c>
+      <c r="J9" s="13">
+        <f t="shared" si="0"/>
+        <v>292712</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="G9" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H9" s="13">
-        <v>1881</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="J9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -2082,22 +2151,29 @@
         <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G10" s="13">
+        <v>297293</v>
+      </c>
+      <c r="H10" s="13">
         <v>294593</v>
       </c>
-      <c r="H10" s="13">
+      <c r="I10" s="13">
         <v>0</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="13">
+        <f t="shared" si="0"/>
+        <v>294593</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L10" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -2112,22 +2188,29 @@
         <v>23</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G11" s="13">
+        <v>297293</v>
+      </c>
+      <c r="H11" s="13">
         <v>294593</v>
       </c>
-      <c r="H11" s="13">
+      <c r="I11" s="13">
         <v>0</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="J11" s="13">
+        <f t="shared" si="0"/>
+        <v>294593</v>
+      </c>
+      <c r="K11" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="4">
+      <c r="L11" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -2136,32 +2219,39 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>262</v>
-      </c>
       <c r="G12" s="13">
+        <v>297293</v>
+      </c>
+      <c r="H12" s="13">
         <v>294593</v>
       </c>
-      <c r="H12" s="13">
+      <c r="I12" s="13">
         <v>263155</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="13">
+        <f t="shared" si="0"/>
+        <v>31438</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -2171,27 +2261,34 @@
         <v>18</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F13" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="G13" s="13">
+      <c r="F13" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="G13" s="47">
+        <v>297293</v>
+      </c>
+      <c r="H13" s="47">
         <v>294593</v>
       </c>
-      <c r="H13" s="13">
+      <c r="I13" s="47">
         <v>66506</v>
       </c>
-      <c r="I13" s="44" t="s">
+      <c r="J13" s="47">
+        <f t="shared" si="0"/>
+        <v>228087</v>
+      </c>
+      <c r="K13" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="J13" s="44" t="s">
+      <c r="L13" s="28" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="2" t="s">
         <v>120</v>
       </c>
@@ -2199,87 +2296,79 @@
         <v>18</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H14" s="13">
-        <v>66506</v>
-      </c>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
+        <v>260</v>
+      </c>
+      <c r="F14" s="23"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H15" s="13">
-        <v>66506</v>
-      </c>
-      <c r="I15" s="45"/>
-      <c r="J15" s="45"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
+        <v>260</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H16" s="13">
-        <v>66506</v>
-      </c>
-      <c r="I16" s="45"/>
-      <c r="J16" s="45"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
+        <v>260</v>
+      </c>
+      <c r="F16" s="23"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H17" s="13">
-        <v>66506</v>
-      </c>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
+        <v>260</v>
+      </c>
+      <c r="F17" s="23"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="2" t="s">
         <v>125</v>
       </c>
@@ -2287,441 +2376,412 @@
         <v>18</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F18" s="20"/>
-      <c r="G18" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H18" s="13">
-        <v>66506</v>
-      </c>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
+        <v>260</v>
+      </c>
+      <c r="F18" s="23"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H19" s="13">
-        <v>66506</v>
-      </c>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="41" t="s">
+        <v>260</v>
+      </c>
+      <c r="F19" s="24"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="19" t="s">
-        <v>297</v>
-      </c>
-      <c r="G20" s="13">
+      <c r="F20" s="22" t="s">
+        <v>294</v>
+      </c>
+      <c r="G20" s="47">
+        <v>297293</v>
+      </c>
+      <c r="H20" s="47">
         <v>294593</v>
       </c>
-      <c r="H20" s="13">
+      <c r="I20" s="47">
         <v>52500</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="J20" s="47">
+        <f t="shared" si="0"/>
+        <v>242093</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="L20" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="42"/>
-      <c r="B21" s="20"/>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="26"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H21" s="13">
-        <v>52500</v>
-      </c>
-      <c r="I21" s="2" t="s">
+      <c r="F21" s="23"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="L21" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="42"/>
-      <c r="B22" s="20"/>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="26"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H22" s="13">
-        <v>52500</v>
-      </c>
-      <c r="I22" s="2" t="s">
+      <c r="F22" s="23"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="L22" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="42"/>
-      <c r="B23" s="20"/>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="26"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H23" s="13">
-        <v>52500</v>
-      </c>
-      <c r="I23" s="2" t="s">
+      <c r="F23" s="23"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="L23" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="42"/>
-      <c r="B24" s="20"/>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="26"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H24" s="13">
-        <v>52500</v>
-      </c>
-      <c r="I24" s="2" t="s">
+      <c r="F24" s="23"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="L24" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="42"/>
-      <c r="B25" s="20"/>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="26"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H25" s="13">
-        <v>52500</v>
-      </c>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="42"/>
-      <c r="B26" s="20"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="26"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H26" s="13">
-        <v>52500</v>
-      </c>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="42"/>
-      <c r="B27" s="20"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="26"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H27" s="13">
-        <v>52500</v>
-      </c>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="42"/>
-      <c r="B28" s="20"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="26"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H28" s="13">
-        <v>52500</v>
-      </c>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="42"/>
-      <c r="B29" s="20"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="26"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F29" s="20"/>
-      <c r="G29" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H29" s="13">
-        <v>52500</v>
-      </c>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="42"/>
-      <c r="B30" s="20"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="26"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H30" s="13">
-        <v>52500</v>
-      </c>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="42"/>
-      <c r="B31" s="20"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="26"/>
+      <c r="B31" s="23"/>
       <c r="C31" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F31" s="20"/>
-      <c r="G31" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H31" s="13">
-        <v>52500</v>
-      </c>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="42"/>
-      <c r="B32" s="20"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="26"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H32" s="13">
-        <v>52500</v>
-      </c>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="42"/>
-      <c r="B33" s="20"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="26"/>
+      <c r="B33" s="23"/>
       <c r="C33" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="20"/>
-      <c r="G33" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H33" s="13">
-        <v>52500</v>
-      </c>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="42"/>
-      <c r="B34" s="20"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="26"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F34" s="20"/>
-      <c r="G34" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H34" s="13">
-        <v>52500</v>
-      </c>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="42"/>
-      <c r="B35" s="20"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="26"/>
+      <c r="B35" s="23"/>
       <c r="C35" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="20"/>
-      <c r="G35" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H35" s="13">
-        <v>52500</v>
-      </c>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="43"/>
-      <c r="B36" s="21"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="27"/>
+      <c r="B36" s="24"/>
       <c r="C36" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F36" s="21"/>
-      <c r="G36" s="13">
-        <v>294593</v>
-      </c>
-      <c r="H36" s="13">
-        <v>52500</v>
-      </c>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F36" s="24"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>15</v>
       </c>
@@ -2736,22 +2796,29 @@
         <v>19</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G37" s="13">
+        <v>297293</v>
+      </c>
+      <c r="H37" s="13">
         <v>294593</v>
       </c>
-      <c r="H37" s="13">
+      <c r="I37" s="13">
         <v>63238</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="J37" s="2" t="s">
+      <c r="J37" s="13">
+        <f t="shared" si="0"/>
+        <v>231355</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="L37" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>16</v>
       </c>
@@ -2760,28 +2827,35 @@
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G38" s="13">
+        <v>297293</v>
+      </c>
+      <c r="H38" s="13">
         <v>294593</v>
       </c>
-      <c r="H38" s="13">
+      <c r="I38" s="13">
         <v>23740</v>
       </c>
-      <c r="I38" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="J38" s="2" t="s">
+      <c r="J38" s="13">
+        <f t="shared" si="0"/>
+        <v>270853</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="L38" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>17</v>
       </c>
@@ -2796,38 +2870,55 @@
         <v>19</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G39" s="13">
+        <v>297293</v>
+      </c>
+      <c r="H39" s="13">
         <v>294593</v>
       </c>
-      <c r="H39" s="13">
+      <c r="I39" s="13">
         <v>0</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="J39" s="13">
+        <f t="shared" si="0"/>
+        <v>294593</v>
+      </c>
+      <c r="K39" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="L39" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B1:J1"/>
+  <mergeCells count="17">
+    <mergeCell ref="J20:J36"/>
+    <mergeCell ref="B1:L1"/>
     <mergeCell ref="B13:B19"/>
     <mergeCell ref="A13:A19"/>
     <mergeCell ref="F13:F19"/>
     <mergeCell ref="A20:A36"/>
     <mergeCell ref="B20:B36"/>
     <mergeCell ref="F20:F36"/>
+    <mergeCell ref="K13:K19"/>
+    <mergeCell ref="L13:L19"/>
+    <mergeCell ref="G13:G19"/>
+    <mergeCell ref="H13:H19"/>
     <mergeCell ref="I13:I19"/>
     <mergeCell ref="J13:J19"/>
+    <mergeCell ref="G20:G36"/>
+    <mergeCell ref="H20:H36"/>
+    <mergeCell ref="I20:I36"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2837,10 +2928,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2851,28 +2942,32 @@
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="38.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.44140625" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="84.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="37.33203125" customWidth="1"/>
+    <col min="10" max="10" width="84.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2886,22 +2981,28 @@
         <v>2</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>273</v>
+        <v>295</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>248</v>
+        <v>296</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>70</v>
       </c>
@@ -2913,21 +3014,28 @@
         <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="F3" s="13">
+        <v>269</v>
+      </c>
+      <c r="F3" s="19">
+        <v>2700000</v>
+      </c>
+      <c r="G3" s="19">
         <f>2700000-76277</f>
         <v>2623723</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="7"/>
+      <c r="I3" s="19">
+        <f>G3-H3</f>
+        <v>2623723</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -2939,21 +3047,28 @@
         <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="F4" s="13">
-        <f t="shared" ref="F4:F11" si="0">2700000-76277</f>
+        <v>270</v>
+      </c>
+      <c r="F4" s="19">
+        <v>2700000</v>
+      </c>
+      <c r="G4" s="19">
+        <f t="shared" ref="G4:G11" si="0">2700000-76277</f>
         <v>2623723</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="7"/>
+      <c r="I4" s="19">
+        <f t="shared" ref="I4:I11" si="1">G4-H4</f>
+        <v>2623723</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>71</v>
       </c>
@@ -2965,21 +3080,28 @@
         <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="F5" s="13">
+        <v>271</v>
+      </c>
+      <c r="F5" s="19">
+        <v>2700000</v>
+      </c>
+      <c r="G5" s="19">
         <f t="shared" si="0"/>
         <v>2623723</v>
       </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="19"/>
+      <c r="I5" s="19">
+        <f t="shared" si="1"/>
+        <v>2623723</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I5" s="12">
+      <c r="K5" s="12">
         <v>1627750414677</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>72</v>
       </c>
@@ -2991,21 +3113,28 @@
         <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="F6" s="13">
+        <v>272</v>
+      </c>
+      <c r="F6" s="19">
+        <v>2700000</v>
+      </c>
+      <c r="G6" s="19">
         <f t="shared" si="0"/>
         <v>2623723</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="7"/>
+      <c r="I6" s="19">
+        <f t="shared" si="1"/>
+        <v>2623723</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>73</v>
       </c>
@@ -3017,23 +3146,30 @@
         <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="F7" s="13">
+        <v>273</v>
+      </c>
+      <c r="F7" s="19">
+        <v>2700000</v>
+      </c>
+      <c r="G7" s="19">
         <f t="shared" si="0"/>
         <v>2623723</v>
       </c>
-      <c r="G7" s="13">
+      <c r="H7" s="19">
         <v>1163823</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="19">
+        <f t="shared" si="1"/>
+        <v>1459900</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>74</v>
       </c>
@@ -3041,33 +3177,40 @@
         <v>76</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="F8" s="13">
+        <v>274</v>
+      </c>
+      <c r="F8" s="19">
+        <v>2700000</v>
+      </c>
+      <c r="G8" s="19">
         <f t="shared" si="0"/>
         <v>2623723</v>
       </c>
-      <c r="G8" s="40">
+      <c r="H8" s="19">
         <v>2530146</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="I8" s="19">
+        <f t="shared" si="1"/>
+        <v>93577</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="K8" s="6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -3077,25 +3220,32 @@
         <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="F9" s="13">
+        <v>271</v>
+      </c>
+      <c r="F9" s="19">
+        <v>2700000</v>
+      </c>
+      <c r="G9" s="19">
         <f t="shared" si="0"/>
         <v>2623723</v>
       </c>
-      <c r="G9" s="13">
+      <c r="H9" s="19">
         <v>2386301</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="19">
+        <f t="shared" si="1"/>
+        <v>237422</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I9" s="12">
+      <c r="K9" s="12">
         <v>628455067818</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29"/>
-      <c r="B10" s="20"/>
+    <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="33"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="2" t="s">
         <v>73</v>
       </c>
@@ -3103,23 +3253,30 @@
         <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="F10" s="13">
+        <v>275</v>
+      </c>
+      <c r="F10" s="19">
+        <v>2700000</v>
+      </c>
+      <c r="G10" s="19">
         <f t="shared" si="0"/>
         <v>2623723</v>
       </c>
-      <c r="G10" s="13">
+      <c r="H10" s="19">
         <v>2386301</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="19">
+        <f t="shared" si="1"/>
+        <v>237422</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>5</v>
       </c>
@@ -3131,21 +3288,28 @@
         <v>18</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F11" s="13">
+        <v>276</v>
+      </c>
+      <c r="F11" s="19">
+        <v>2700000</v>
+      </c>
+      <c r="G11" s="19">
         <f t="shared" si="0"/>
         <v>2623723</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="7"/>
+      <c r="I11" s="19">
+        <f t="shared" si="1"/>
+        <v>2623723</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3154,9 +3318,11 @@
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3166,8 +3332,10 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3177,8 +3345,10 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -3186,10 +3356,12 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -3197,10 +3369,12 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -3208,10 +3382,12 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -3219,10 +3395,12 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -3230,10 +3408,12 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -3243,8 +3423,10 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3254,8 +3436,10 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3265,10 +3449,12 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B1:K1"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="A9:A10"/>
   </mergeCells>
@@ -3298,14 +3484,14 @@
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -3540,10 +3726,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="36" t="s">
         <v>116</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -3561,9 +3747,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="30"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="20" t="s">
+      <c r="A15" s="34"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="23" t="s">
         <v>106</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -3580,9 +3766,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="30"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="20"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="2" t="s">
         <v>108</v>
       </c>
@@ -3597,9 +3783,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="30"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="20"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="2" t="s">
         <v>109</v>
       </c>
@@ -3614,9 +3800,9 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="30"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="20"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="2" t="s">
         <v>110</v>
       </c>
@@ -3631,9 +3817,9 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="30"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="21"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="2" t="s">
         <v>111</v>
       </c>
@@ -3667,10 +3853,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="39" t="s">
         <v>116</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -3686,8 +3872,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="30"/>
-      <c r="B22" s="32"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="39"/>
       <c r="C22" s="3" t="s">
         <v>120</v>
       </c>
@@ -3695,7 +3881,7 @@
       <c r="E22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="30" t="s">
+      <c r="F22" s="34" t="s">
         <v>144</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -3703,8 +3889,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="30"/>
-      <c r="B23" s="32"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="39"/>
       <c r="C23" s="3" t="s">
         <v>121</v>
       </c>
@@ -3712,14 +3898,14 @@
       <c r="E23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="30"/>
+      <c r="F23" s="34"/>
       <c r="G23" s="2" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="30"/>
-      <c r="B24" s="32"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="39"/>
       <c r="C24" s="3" t="s">
         <v>122</v>
       </c>
@@ -3727,14 +3913,14 @@
       <c r="E24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="30"/>
+      <c r="F24" s="34"/>
       <c r="G24" s="2" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="30"/>
-      <c r="B25" s="32"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="39"/>
       <c r="C25" s="3" t="s">
         <v>123</v>
       </c>
@@ -3742,14 +3928,14 @@
       <c r="E25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="30"/>
+      <c r="F25" s="34"/>
       <c r="G25" s="2" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="30"/>
-      <c r="B26" s="32"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="39"/>
       <c r="C26" s="3" t="s">
         <v>124</v>
       </c>
@@ -3757,14 +3943,14 @@
       <c r="E26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="30"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="2" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="30"/>
-      <c r="B27" s="32"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="39"/>
       <c r="C27" s="3" t="s">
         <v>125</v>
       </c>
@@ -3772,7 +3958,7 @@
       <c r="E27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="30"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="2" t="s">
         <v>157</v>
       </c>
@@ -3812,12 +3998,12 @@
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -4081,12 +4267,12 @@
       <c r="A1" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -4519,12 +4705,12 @@
       <c r="A1" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -4765,12 +4951,12 @@
       <c r="A1" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -4917,10 +5103,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="41" t="s">
         <v>186</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="41"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
@@ -4953,10 +5139,10 @@
       <c r="B8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="42" t="s">
         <v>187</v>
       </c>
       <c r="M8" s="5" t="s">
@@ -5129,10 +5315,10 @@
       <c r="N22" s="1"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="P25" s="38" t="s">
+      <c r="P25" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="Q25" s="39"/>
+      <c r="Q25" s="46"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P26" s="1" t="s">
@@ -5161,14 +5347,14 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="G30" s="36" t="s">
+      <c r="G30" s="43" t="s">
         <v>188</v>
       </c>
-      <c r="H30" s="37"/>
-      <c r="J30" s="38" t="s">
+      <c r="H30" s="44"/>
+      <c r="J30" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="K30" s="39"/>
+      <c r="K30" s="46"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="2" t="s">
         <v>166</v>
@@ -5276,10 +5462,10 @@
       <c r="H38" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="J38" s="34" t="s">
+      <c r="J38" s="41" t="s">
         <v>212</v>
       </c>
-      <c r="K38" s="34"/>
+      <c r="K38" s="41"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="2" t="s">
         <v>236</v>

</xml_diff>